<commit_message>
update: new MEG model runs
</commit_message>
<xml_diff>
--- a/scripts_reproducibility/run_orders.xlsx
+++ b/scripts_reproducibility/run_orders.xlsx
@@ -112,7 +112,7 @@
     <t>[4,2,6,1,3,0,7,5]</t>
   </si>
   <si>
-    <t>[2,3,5,1,7,6,4,0]</t>
+    <t>[0,6,2,5,7,3,4,1]</t>
   </si>
   <si>
     <t>[5,4,2,3,0,7,1,6]</t>
@@ -130,34 +130,34 @@
     <t>[7,6,0,5,4,2,3,1]</t>
   </si>
   <si>
-    <t>[0,3,7,1,4,2,6,5]</t>
-  </si>
-  <si>
-    <t>[3,5,2,1,6,7,4,0]</t>
-  </si>
-  <si>
-    <t>[6,2,5,0,4,3,7,1]</t>
-  </si>
-  <si>
-    <t>[7,3,0,1,4,2,5,6]</t>
-  </si>
-  <si>
-    <t>[5,7,3,0,6,2,1,4]</t>
-  </si>
-  <si>
-    <t>[7,5,0,2,1,4,3,6]</t>
-  </si>
-  <si>
-    <t>[3,5,0,2,7,6,1,4]</t>
-  </si>
-  <si>
-    <t>[7,3,0,1,6,4,2,5]</t>
-  </si>
-  <si>
-    <t>[3,7,1,4,6,0,2,5]</t>
-  </si>
-  <si>
-    <t>[2,6,5,1,7,3,4,0]</t>
+    <t>[0,3,6,1,4,2,7,5]</t>
+  </si>
+  <si>
+    <t>[3,5,4,1,6,7,2,0]</t>
+  </si>
+  <si>
+    <t>[6,2,7,0,4,3,5,1]</t>
+  </si>
+  <si>
+    <t>[7,3,5,1,4,2,0,6]</t>
+  </si>
+  <si>
+    <t>[5,7,1,0,6,2,3,4]</t>
+  </si>
+  <si>
+    <t>[7,5,3,2,1,4,0,6]</t>
+  </si>
+  <si>
+    <t>[3,5,1,2,7,6,0,4]</t>
+  </si>
+  <si>
+    <t>[7,3,2,1,6,4,0,5]</t>
+  </si>
+  <si>
+    <t>[3,7,2,4,6,0,1,5]</t>
+  </si>
+  <si>
+    <t>[2,6,4,1,7,3,5,0]</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="2">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>32</v>

</xml_diff>